<commit_message>
* Update database pagination * Add user website
</commit_message>
<xml_diff>
--- a/GoosEnterprise.Model/DBScript/Pladis 2020.xlsx
+++ b/GoosEnterprise.Model/DBScript/Pladis 2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muniram\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karthik\Downloads\GoodsEnterprise\GoosEnterprise.Model\DBScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E034FE-F07E-453F-8357-C7EC4ADE9460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79787C97-2B80-46CD-BE50-EB4DB7A89BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1692,35 +1692,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F268" workbookViewId="0">
-      <selection activeCell="G111" sqref="G111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.44140625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="14.5546875" style="8" customWidth="1"/>
-    <col min="16" max="16" width="18.21875" style="8" customWidth="1"/>
-    <col min="17" max="17" width="20" style="8" customWidth="1"/>
-    <col min="18" max="18" width="16.21875" style="10" customWidth="1"/>
-    <col min="19" max="19" width="17.88671875" style="10" customWidth="1"/>
-    <col min="20" max="20" width="15.77734375" style="10" customWidth="1"/>
-    <col min="21" max="21" width="17.88671875" style="10" customWidth="1"/>
-    <col min="22" max="22" width="15.21875" style="6" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" style="6" customWidth="1"/>
-    <col min="24" max="24" width="16.5546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="15.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="16" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.109375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>